<commit_message>
tei 0.2.0 con SR arreglado 3 de junio
</commit_message>
<xml_diff>
--- a/fhir/ig/tei/0.2.0/StructureDefinition-PrestadorAdministrativoLE.xlsx
+++ b/fhir/ig/tei/0.2.0/StructureDefinition-PrestadorAdministrativoLE.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$242</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8798" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8762" uniqueCount="809">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-31T16:50:11-04:00</t>
+    <t>2024-06-03T10:40:28-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2463,12 +2463,6 @@
   </si>
   <si>
     <t>Practitioner.qualification:SubEsp.issuer.display</t>
-  </si>
-  <si>
-    <t>Practitioner.qualification:TituloProfesional</t>
-  </si>
-  <si>
-    <t>TituloProfesional</t>
   </si>
   <si>
     <t>Practitioner.qualification:EspecialidadMedica</t>
@@ -2824,7 +2818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN243"/>
+  <dimension ref="A1:AN242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -17968,7 +17962,7 @@
         <v>78</v>
       </c>
       <c r="G133" t="s" s="2">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H133" t="s" s="2">
         <v>89</v>
@@ -30162,7 +30156,7 @@
         <v>78</v>
       </c>
       <c r="G240" t="s" s="2">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H240" t="s" s="2">
         <v>89</v>
@@ -30377,11 +30371,9 @@
         <v>801</v>
       </c>
       <c r="B242" t="s" s="2">
-        <v>585</v>
-      </c>
-      <c r="C242" t="s" s="2">
-        <v>802</v>
-      </c>
+        <v>801</v>
+      </c>
+      <c r="C242" s="2"/>
       <c r="D242" t="s" s="2">
         <v>77</v>
       </c>
@@ -30390,10 +30382,10 @@
         <v>78</v>
       </c>
       <c r="G242" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H242" t="s" s="2">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I242" t="s" s="2">
         <v>77</v>
@@ -30402,16 +30394,20 @@
         <v>77</v>
       </c>
       <c r="K242" t="s" s="2">
-        <v>586</v>
+        <v>188</v>
       </c>
       <c r="L242" t="s" s="2">
-        <v>587</v>
+        <v>802</v>
       </c>
       <c r="M242" t="s" s="2">
-        <v>588</v>
-      </c>
-      <c r="N242" s="2"/>
-      <c r="O242" s="2"/>
+        <v>803</v>
+      </c>
+      <c r="N242" t="s" s="2">
+        <v>804</v>
+      </c>
+      <c r="O242" t="s" s="2">
+        <v>805</v>
+      </c>
       <c r="P242" t="s" s="2">
         <v>77</v>
       </c>
@@ -30435,13 +30431,13 @@
         <v>77</v>
       </c>
       <c r="X242" t="s" s="2">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="Y242" t="s" s="2">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="Z242" t="s" s="2">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="AA242" t="s" s="2">
         <v>77</v>
@@ -30459,7 +30455,7 @@
         <v>77</v>
       </c>
       <c r="AF242" t="s" s="2">
-        <v>585</v>
+        <v>801</v>
       </c>
       <c r="AG242" t="s" s="2">
         <v>78</v>
@@ -30474,136 +30470,20 @@
         <v>100</v>
       </c>
       <c r="AK242" t="s" s="2">
-        <v>591</v>
+        <v>806</v>
       </c>
       <c r="AL242" t="s" s="2">
-        <v>592</v>
+        <v>807</v>
       </c>
       <c r="AM242" t="s" s="2">
-        <v>593</v>
+        <v>808</v>
       </c>
       <c r="AN242" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="243" hidden="true">
-      <c r="A243" t="s" s="2">
-        <v>803</v>
-      </c>
-      <c r="B243" t="s" s="2">
-        <v>803</v>
-      </c>
-      <c r="C243" s="2"/>
-      <c r="D243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E243" s="2"/>
-      <c r="F243" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G243" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K243" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="L243" t="s" s="2">
-        <v>804</v>
-      </c>
-      <c r="M243" t="s" s="2">
-        <v>805</v>
-      </c>
-      <c r="N243" t="s" s="2">
-        <v>806</v>
-      </c>
-      <c r="O243" t="s" s="2">
-        <v>807</v>
-      </c>
-      <c r="P243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q243" s="2"/>
-      <c r="R243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X243" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="Y243" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="Z243" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AA243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF243" t="s" s="2">
-        <v>803</v>
-      </c>
-      <c r="AG243" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH243" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI243" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ243" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AK243" t="s" s="2">
-        <v>808</v>
-      </c>
-      <c r="AL243" t="s" s="2">
-        <v>809</v>
-      </c>
-      <c r="AM243" t="s" s="2">
-        <v>810</v>
-      </c>
-      <c r="AN243" t="s" s="2">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN243">
+  <autoFilter ref="A1:AN242">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -30613,7 +30493,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI242">
+  <conditionalFormatting sqref="A2:AI241">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>